<commit_message>
New files and graphs from new model of photoreceptor generation.
</commit_message>
<xml_diff>
--- a/Retina Project Beta/Photoreceptor Generation.tsv.xlsx
+++ b/Retina Project Beta/Photoreceptor Generation.tsv.xlsx
@@ -15,39 +15,11 @@
     <sheet name="coneGeneration" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">coneGeneration!$B$1:$B$7951</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">coneGeneration!$A$1:$A$694</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">coneGeneration!$J$1:$J$694</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">coneGeneration!$K$1:$K$694</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">coneGeneration!$L$1:$L$694</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">coneGeneration!$M$1:$M$694</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">coneGeneration!$N$1:$N$694</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">coneGeneration!$O$1:$O$694</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">coneGeneration!$P$1:$P$694</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">coneGeneration!$Q$1:$Q$694</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">coneGeneration!$R$1:$R$694</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">coneGeneration!$S$1:$S$694</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">coneGeneration!$B$1:$B$694</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">coneGeneration!$T$1:$T$694</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">coneGeneration!$U$1:$U$694</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">coneGeneration!$V$1:$V$694</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">coneGeneration!$A$1:$A$7951</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">coneGeneration!$B$1:$B$7951</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">coneGeneration!$B$1:$B$7951</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">coneGeneration!$C$1:$C$694</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">coneGeneration!$D$1:$D$694</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">coneGeneration!$E$1:$E$694</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">coneGeneration!$F$1:$F$694</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">coneGeneration!$G$1:$G$694</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">coneGeneration!$H$1:$H$694</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">coneGeneration!$I$1:$I$694</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">coneGeneration!$A$1:$A$7951</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">coneGeneration!$B$1:$B$7951</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -602,7 +574,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.23</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -700,7 +672,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2345,7 +2317,7 @@
   <dimension ref="A1:B7951"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>